<commit_message>
20240715 Actualizacion ultimas predicciones (csv y metricas)
</commit_message>
<xml_diff>
--- a/013_metrics_summary.xlsx
+++ b/013_metrics_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aure/acGdrive/00_Aure/AWS/00-UAustral/03-Grupos/Labo3-Denicolay/77_TP_Entrega_Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A826D-4554-7343-BFAA-EEC4F19701B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D49AA6-871F-DF4E-A7B4-E358C4E9685B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="41260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
   <si>
     <t>file_name</t>
   </si>
@@ -668,6 +668,99 @@
   </si>
   <si>
     <t>20240714-1708-LSTM_v8v4_feb_tfe2_0.309.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2152-LSTM_v8v4_feb_tfe2_0.3826.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2156-LSTM_v8v4_feb_tfe2_0.3995.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2159-LSTM_v8v4_feb_tfe2_0.3876.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2204-LSTM_v8v4_feb_tfe2_0.3743.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2314-LSTM_v8v4_feb_tfe2_0.3431.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2322-LSTM_v8v4_feb_tfe2_0.2775.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2327-LSTM_v8v4_feb_tfe2_0.3218.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2334-LSTM_v8v4_feb_tfe2_0.2988.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2344-LSTM_v8v4_feb_tfe2_0.2942.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2351-LSTM_v8v4_feb_tfe2_0.2847.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240714-2357-LSTM_v8v4_feb_tfe2_0.2996.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0008-LSTM_v8v4_feb_tfe2_0.3168.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0016-LSTM_v8v4_feb_tfe2_0.3185.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0025-LSTM_v8v4_feb_tfe2_0.3231.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0034-LSTM_v8v4_feb_tfe2_0.3119.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0046-LSTM_v8v4_feb_tfe2_0.287.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0100-LSTM_v8v4_feb_tfe2_0.3029.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0117-LSTM_v8v4_feb_tfe2_0.316.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0133-LSTM_v8v4_feb_tfe2_0.2833.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0145-LSTM_v8v4_feb_tfe2_0.2692.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0201-LSTM_v8v4_feb_tfe2_0.2931.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0219-LSTM_v8v4_feb_tfe2_0.2931.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0237-LSTM_v8v4_feb_tfe2_0.2738.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0251-LSTM_v8v4_feb_tfe2_0.2724.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0305-LSTM_v8v4_feb_tfe2_0.2969.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0322-LSTM_v8v4_feb_tfe2_0.289.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0340-LSTM_v8v4_feb_tfe2_0.2979.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0352-LSTM_v8v4_feb_tfe2_0.2699.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0408-LSTM_v8v4_feb_tfe2_0.2911.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0426-LSTM_v8v4_feb_tfe2_0.286.csv.metrics.json</t>
+  </si>
+  <si>
+    <t>20240715-0446-LSTM_v8v4_feb_tfe2_0.284.csv.metrics.json</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R199"/>
+  <dimension ref="A1:R230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12187,6 +12280,1742 @@
         <v>0.29118245198917708</v>
       </c>
     </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>216</v>
+      </c>
+      <c r="B200" t="b">
+        <v>1</v>
+      </c>
+      <c r="C200">
+        <v>52</v>
+      </c>
+      <c r="D200">
+        <v>12</v>
+      </c>
+      <c r="E200">
+        <v>150</v>
+      </c>
+      <c r="F200">
+        <v>64</v>
+      </c>
+      <c r="G200">
+        <v>1E-4</v>
+      </c>
+      <c r="H200">
+        <v>10</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <v>1</v>
+      </c>
+      <c r="K200">
+        <v>4.3538456545269302</v>
+      </c>
+      <c r="L200">
+        <v>10.65364500026341</v>
+      </c>
+      <c r="M200">
+        <v>157.63699173423981</v>
+      </c>
+      <c r="N200">
+        <v>0.38256401328100093</v>
+      </c>
+      <c r="O200">
+        <v>4.3538456545269293</v>
+      </c>
+      <c r="P200">
+        <v>12.53124331686613</v>
+      </c>
+      <c r="Q200">
+        <v>157.63699173423981</v>
+      </c>
+      <c r="R200">
+        <v>0.3207912364753614</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>217</v>
+      </c>
+      <c r="B201" t="b">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <v>52</v>
+      </c>
+      <c r="D201">
+        <v>12</v>
+      </c>
+      <c r="E201">
+        <v>150</v>
+      </c>
+      <c r="F201">
+        <v>64</v>
+      </c>
+      <c r="G201">
+        <v>1E-4</v>
+      </c>
+      <c r="H201">
+        <v>20</v>
+      </c>
+      <c r="I201">
+        <v>0</v>
+      </c>
+      <c r="J201">
+        <v>1</v>
+      </c>
+      <c r="K201">
+        <v>4.6315843278595494</v>
+      </c>
+      <c r="L201">
+        <v>11.144032149398321</v>
+      </c>
+      <c r="M201">
+        <v>169.50317233622721</v>
+      </c>
+      <c r="N201">
+        <v>0.39954439910918599</v>
+      </c>
+      <c r="O201">
+        <v>4.6315843278595494</v>
+      </c>
+      <c r="P201">
+        <v>13.22694766430044</v>
+      </c>
+      <c r="Q201">
+        <v>169.50317233622721</v>
+      </c>
+      <c r="R201">
+        <v>0.34211227117098542</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>218</v>
+      </c>
+      <c r="B202" t="b">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <v>11</v>
+      </c>
+      <c r="D202">
+        <v>12</v>
+      </c>
+      <c r="E202">
+        <v>150</v>
+      </c>
+      <c r="F202">
+        <v>64</v>
+      </c>
+      <c r="G202">
+        <v>1E-4</v>
+      </c>
+      <c r="H202">
+        <v>10</v>
+      </c>
+      <c r="I202">
+        <v>0</v>
+      </c>
+      <c r="J202">
+        <v>1</v>
+      </c>
+      <c r="K202">
+        <v>4.3751335809332996</v>
+      </c>
+      <c r="L202">
+        <v>10.529316256944851</v>
+      </c>
+      <c r="M202">
+        <v>158.74727758611371</v>
+      </c>
+      <c r="N202">
+        <v>0.3876042783016202</v>
+      </c>
+      <c r="O202">
+        <v>4.3751335809332996</v>
+      </c>
+      <c r="P202">
+        <v>12.360251918398509</v>
+      </c>
+      <c r="Q202">
+        <v>158.7472775861138</v>
+      </c>
+      <c r="R202">
+        <v>0.32189843948235147</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>219</v>
+      </c>
+      <c r="B203" t="b">
+        <v>1</v>
+      </c>
+      <c r="C203">
+        <v>11</v>
+      </c>
+      <c r="D203">
+        <v>12</v>
+      </c>
+      <c r="E203">
+        <v>150</v>
+      </c>
+      <c r="F203">
+        <v>64</v>
+      </c>
+      <c r="G203">
+        <v>1E-4</v>
+      </c>
+      <c r="H203">
+        <v>20</v>
+      </c>
+      <c r="I203">
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <v>1</v>
+      </c>
+      <c r="K203">
+        <v>4.3339827204079064</v>
+      </c>
+      <c r="L203">
+        <v>11.147491161963289</v>
+      </c>
+      <c r="M203">
+        <v>147.76321685757969</v>
+      </c>
+      <c r="N203">
+        <v>0.37433821115165189</v>
+      </c>
+      <c r="O203">
+        <v>4.3339827204079047</v>
+      </c>
+      <c r="P203">
+        <v>13.52096924002184</v>
+      </c>
+      <c r="Q203">
+        <v>147.76321685757969</v>
+      </c>
+      <c r="R203">
+        <v>0.31829039388317981</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>220</v>
+      </c>
+      <c r="B204" t="b">
+        <v>1</v>
+      </c>
+      <c r="C204">
+        <v>52</v>
+      </c>
+      <c r="D204">
+        <v>12</v>
+      </c>
+      <c r="E204">
+        <v>150</v>
+      </c>
+      <c r="F204">
+        <v>64</v>
+      </c>
+      <c r="G204">
+        <v>1E-4</v>
+      </c>
+      <c r="H204">
+        <v>10</v>
+      </c>
+      <c r="I204">
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <v>0</v>
+      </c>
+      <c r="K204">
+        <v>4.8618613824094608</v>
+      </c>
+      <c r="L204">
+        <v>10.65364069541036</v>
+      </c>
+      <c r="M204">
+        <v>117.16911619972019</v>
+      </c>
+      <c r="N204">
+        <v>0.3431243960673912</v>
+      </c>
+      <c r="O204">
+        <v>4.8618613824094608</v>
+      </c>
+      <c r="P204">
+        <v>12.4825992908528</v>
+      </c>
+      <c r="Q204">
+        <v>117.16911619972009</v>
+      </c>
+      <c r="R204">
+        <v>0.35968772385193648</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>221</v>
+      </c>
+      <c r="B205" t="b">
+        <v>1</v>
+      </c>
+      <c r="C205">
+        <v>52</v>
+      </c>
+      <c r="D205">
+        <v>12</v>
+      </c>
+      <c r="E205">
+        <v>150</v>
+      </c>
+      <c r="F205">
+        <v>64</v>
+      </c>
+      <c r="G205">
+        <v>1E-4</v>
+      </c>
+      <c r="H205">
+        <v>20</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>0</v>
+      </c>
+      <c r="K205">
+        <v>3.4634401086203579</v>
+      </c>
+      <c r="L205">
+        <v>9.0624573912117068</v>
+      </c>
+      <c r="M205">
+        <v>101.613043772823</v>
+      </c>
+      <c r="N205">
+        <v>0.2775418722793469</v>
+      </c>
+      <c r="O205">
+        <v>3.4634401086203579</v>
+      </c>
+      <c r="P205">
+        <v>10.68154411394824</v>
+      </c>
+      <c r="Q205">
+        <v>101.6130437728231</v>
+      </c>
+      <c r="R205">
+        <v>0.25575739711712708</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>222</v>
+      </c>
+      <c r="B206" t="b">
+        <v>1</v>
+      </c>
+      <c r="C206">
+        <v>11</v>
+      </c>
+      <c r="D206">
+        <v>12</v>
+      </c>
+      <c r="E206">
+        <v>150</v>
+      </c>
+      <c r="F206">
+        <v>64</v>
+      </c>
+      <c r="G206">
+        <v>1E-4</v>
+      </c>
+      <c r="H206">
+        <v>10</v>
+      </c>
+      <c r="I206">
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+      <c r="K206">
+        <v>4.2638825680477321</v>
+      </c>
+      <c r="L206">
+        <v>10.14999079023832</v>
+      </c>
+      <c r="M206">
+        <v>108.30726244811621</v>
+      </c>
+      <c r="N206">
+        <v>0.32180587097787799</v>
+      </c>
+      <c r="O206">
+        <v>4.263882568047733</v>
+      </c>
+      <c r="P206">
+        <v>11.96770717352959</v>
+      </c>
+      <c r="Q206">
+        <v>108.30726244811621</v>
+      </c>
+      <c r="R206">
+        <v>0.3137701243338753</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>223</v>
+      </c>
+      <c r="B207" t="b">
+        <v>1</v>
+      </c>
+      <c r="C207">
+        <v>11</v>
+      </c>
+      <c r="D207">
+        <v>12</v>
+      </c>
+      <c r="E207">
+        <v>150</v>
+      </c>
+      <c r="F207">
+        <v>64</v>
+      </c>
+      <c r="G207">
+        <v>1E-4</v>
+      </c>
+      <c r="H207">
+        <v>20</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+      <c r="K207">
+        <v>3.9156614242367498</v>
+      </c>
+      <c r="L207">
+        <v>9.9356815993460348</v>
+      </c>
+      <c r="M207">
+        <v>104.8847162741561</v>
+      </c>
+      <c r="N207">
+        <v>0.29883902648852018</v>
+      </c>
+      <c r="O207">
+        <v>3.9156614242367498</v>
+      </c>
+      <c r="P207">
+        <v>11.664003298640891</v>
+      </c>
+      <c r="Q207">
+        <v>104.8847162741562</v>
+      </c>
+      <c r="R207">
+        <v>0.28855921800384071</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>224</v>
+      </c>
+      <c r="B208" t="b">
+        <v>1</v>
+      </c>
+      <c r="C208">
+        <v>52</v>
+      </c>
+      <c r="D208">
+        <v>3</v>
+      </c>
+      <c r="E208">
+        <v>150</v>
+      </c>
+      <c r="F208">
+        <v>64</v>
+      </c>
+      <c r="G208">
+        <v>1E-4</v>
+      </c>
+      <c r="H208">
+        <v>20</v>
+      </c>
+      <c r="I208">
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <v>0</v>
+      </c>
+      <c r="K208">
+        <v>3.826123015163716</v>
+      </c>
+      <c r="L208">
+        <v>9.9102863868318529</v>
+      </c>
+      <c r="M208">
+        <v>114.04400677885749</v>
+      </c>
+      <c r="N208">
+        <v>0.29419929121211541</v>
+      </c>
+      <c r="O208">
+        <v>3.826123015163716</v>
+      </c>
+      <c r="P208">
+        <v>11.631603978529631</v>
+      </c>
+      <c r="Q208">
+        <v>114.04400677885739</v>
+      </c>
+      <c r="R208">
+        <v>0.27602694629923519</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>225</v>
+      </c>
+      <c r="B209" t="b">
+        <v>1</v>
+      </c>
+      <c r="C209">
+        <v>52</v>
+      </c>
+      <c r="D209">
+        <v>6</v>
+      </c>
+      <c r="E209">
+        <v>150</v>
+      </c>
+      <c r="F209">
+        <v>64</v>
+      </c>
+      <c r="G209">
+        <v>1E-4</v>
+      </c>
+      <c r="H209">
+        <v>20</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <v>0</v>
+      </c>
+      <c r="K209">
+        <v>3.5337030753467462</v>
+      </c>
+      <c r="L209">
+        <v>8.9720167171674472</v>
+      </c>
+      <c r="M209">
+        <v>114.78278127237201</v>
+      </c>
+      <c r="N209">
+        <v>0.28470519036120379</v>
+      </c>
+      <c r="O209">
+        <v>3.5337030753467449</v>
+      </c>
+      <c r="P209">
+        <v>10.309668425167979</v>
+      </c>
+      <c r="Q209">
+        <v>114.78278127237201</v>
+      </c>
+      <c r="R209">
+        <v>0.25785849272758599</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>226</v>
+      </c>
+      <c r="B210" t="b">
+        <v>1</v>
+      </c>
+      <c r="C210">
+        <v>52</v>
+      </c>
+      <c r="D210">
+        <v>9</v>
+      </c>
+      <c r="E210">
+        <v>150</v>
+      </c>
+      <c r="F210">
+        <v>64</v>
+      </c>
+      <c r="G210">
+        <v>1E-4</v>
+      </c>
+      <c r="H210">
+        <v>20</v>
+      </c>
+      <c r="I210">
+        <v>0</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
+      </c>
+      <c r="K210">
+        <v>3.7998584198598522</v>
+      </c>
+      <c r="L210">
+        <v>9.5305291588702179</v>
+      </c>
+      <c r="M210">
+        <v>110.9883995758892</v>
+      </c>
+      <c r="N210">
+        <v>0.29962336828946179</v>
+      </c>
+      <c r="O210">
+        <v>3.7998584198598522</v>
+      </c>
+      <c r="P210">
+        <v>11.156696166880639</v>
+      </c>
+      <c r="Q210">
+        <v>110.9883995758892</v>
+      </c>
+      <c r="R210">
+        <v>0.27791478385879331</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>227</v>
+      </c>
+      <c r="B211" t="b">
+        <v>1</v>
+      </c>
+      <c r="C211">
+        <v>52</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+      <c r="E211">
+        <v>16</v>
+      </c>
+      <c r="F211">
+        <v>8</v>
+      </c>
+      <c r="G211">
+        <v>1E-4</v>
+      </c>
+      <c r="H211">
+        <v>20</v>
+      </c>
+      <c r="I211">
+        <v>0</v>
+      </c>
+      <c r="J211">
+        <v>0</v>
+      </c>
+      <c r="K211">
+        <v>3.826829036785659</v>
+      </c>
+      <c r="L211">
+        <v>9.5293095879935183</v>
+      </c>
+      <c r="M211">
+        <v>154.69638718553139</v>
+      </c>
+      <c r="N211">
+        <v>0.31682778408909162</v>
+      </c>
+      <c r="O211">
+        <v>3.826829036785659</v>
+      </c>
+      <c r="P211">
+        <v>11.22099266582515</v>
+      </c>
+      <c r="Q211">
+        <v>154.69638718553139</v>
+      </c>
+      <c r="R211">
+        <v>0.2762652644187128</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>228</v>
+      </c>
+      <c r="B212" t="b">
+        <v>1</v>
+      </c>
+      <c r="C212">
+        <v>52</v>
+      </c>
+      <c r="D212">
+        <v>6</v>
+      </c>
+      <c r="E212">
+        <v>16</v>
+      </c>
+      <c r="F212">
+        <v>8</v>
+      </c>
+      <c r="G212">
+        <v>1E-4</v>
+      </c>
+      <c r="H212">
+        <v>20</v>
+      </c>
+      <c r="I212">
+        <v>0</v>
+      </c>
+      <c r="J212">
+        <v>0</v>
+      </c>
+      <c r="K212">
+        <v>3.962331930921382</v>
+      </c>
+      <c r="L212">
+        <v>10.275005332370791</v>
+      </c>
+      <c r="M212">
+        <v>139.96372437454849</v>
+      </c>
+      <c r="N212">
+        <v>0.31851198990030027</v>
+      </c>
+      <c r="O212">
+        <v>3.962331930921382</v>
+      </c>
+      <c r="P212">
+        <v>12.49412506186963</v>
+      </c>
+      <c r="Q212">
+        <v>139.96372437454849</v>
+      </c>
+      <c r="R212">
+        <v>0.29104962387186778</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>229</v>
+      </c>
+      <c r="B213" t="b">
+        <v>1</v>
+      </c>
+      <c r="C213">
+        <v>52</v>
+      </c>
+      <c r="D213">
+        <v>9</v>
+      </c>
+      <c r="E213">
+        <v>16</v>
+      </c>
+      <c r="F213">
+        <v>8</v>
+      </c>
+      <c r="G213">
+        <v>1E-4</v>
+      </c>
+      <c r="H213">
+        <v>20</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+      <c r="J213">
+        <v>0</v>
+      </c>
+      <c r="K213">
+        <v>4.0445427949546362</v>
+      </c>
+      <c r="L213">
+        <v>10.2047964709787</v>
+      </c>
+      <c r="M213">
+        <v>125.41679154430641</v>
+      </c>
+      <c r="N213">
+        <v>0.32312743687785189</v>
+      </c>
+      <c r="O213">
+        <v>4.0445427949546362</v>
+      </c>
+      <c r="P213">
+        <v>12.27840427759936</v>
+      </c>
+      <c r="Q213">
+        <v>125.41679154430641</v>
+      </c>
+      <c r="R213">
+        <v>0.29796602566689151</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>230</v>
+      </c>
+      <c r="B214" t="b">
+        <v>1</v>
+      </c>
+      <c r="C214">
+        <v>52</v>
+      </c>
+      <c r="D214">
+        <v>12</v>
+      </c>
+      <c r="E214">
+        <v>16</v>
+      </c>
+      <c r="F214">
+        <v>8</v>
+      </c>
+      <c r="G214">
+        <v>1E-4</v>
+      </c>
+      <c r="H214">
+        <v>20</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+      <c r="K214">
+        <v>4.0827227424962116</v>
+      </c>
+      <c r="L214">
+        <v>10.685479756777809</v>
+      </c>
+      <c r="M214">
+        <v>105.9006753767575</v>
+      </c>
+      <c r="N214">
+        <v>0.31188722096146171</v>
+      </c>
+      <c r="O214">
+        <v>4.0827227424962116</v>
+      </c>
+      <c r="P214">
+        <v>13.35791992146115</v>
+      </c>
+      <c r="Q214">
+        <v>105.9006753767575</v>
+      </c>
+      <c r="R214">
+        <v>0.30190150498455409</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>231</v>
+      </c>
+      <c r="B215" t="b">
+        <v>1</v>
+      </c>
+      <c r="C215">
+        <v>52</v>
+      </c>
+      <c r="D215">
+        <v>3</v>
+      </c>
+      <c r="E215">
+        <v>32</v>
+      </c>
+      <c r="F215">
+        <v>8</v>
+      </c>
+      <c r="G215">
+        <v>1E-4</v>
+      </c>
+      <c r="H215">
+        <v>20</v>
+      </c>
+      <c r="I215">
+        <v>0</v>
+      </c>
+      <c r="J215">
+        <v>0</v>
+      </c>
+      <c r="K215">
+        <v>3.687045966012128</v>
+      </c>
+      <c r="L215">
+        <v>8.8205560035476562</v>
+      </c>
+      <c r="M215">
+        <v>114.2519296756148</v>
+      </c>
+      <c r="N215">
+        <v>0.28703890904599721</v>
+      </c>
+      <c r="O215">
+        <v>3.687045966012128</v>
+      </c>
+      <c r="P215">
+        <v>10.14082790311549</v>
+      </c>
+      <c r="Q215">
+        <v>114.2519296756148</v>
+      </c>
+      <c r="R215">
+        <v>0.2646854696035274</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>232</v>
+      </c>
+      <c r="B216" t="b">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>52</v>
+      </c>
+      <c r="D216">
+        <v>6</v>
+      </c>
+      <c r="E216">
+        <v>32</v>
+      </c>
+      <c r="F216">
+        <v>8</v>
+      </c>
+      <c r="G216">
+        <v>1E-4</v>
+      </c>
+      <c r="H216">
+        <v>20</v>
+      </c>
+      <c r="I216">
+        <v>0</v>
+      </c>
+      <c r="J216">
+        <v>0</v>
+      </c>
+      <c r="K216">
+        <v>3.7919195922083881</v>
+      </c>
+      <c r="L216">
+        <v>9.4286646953347883</v>
+      </c>
+      <c r="M216">
+        <v>140.81943290750399</v>
+      </c>
+      <c r="N216">
+        <v>0.3028880209412072</v>
+      </c>
+      <c r="O216">
+        <v>3.7919195922083868</v>
+      </c>
+      <c r="P216">
+        <v>11.0797090581119</v>
+      </c>
+      <c r="Q216">
+        <v>140.81943290750399</v>
+      </c>
+      <c r="R216">
+        <v>0.27505930665826711</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>233</v>
+      </c>
+      <c r="B217" t="b">
+        <v>1</v>
+      </c>
+      <c r="C217">
+        <v>52</v>
+      </c>
+      <c r="D217">
+        <v>9</v>
+      </c>
+      <c r="E217">
+        <v>32</v>
+      </c>
+      <c r="F217">
+        <v>8</v>
+      </c>
+      <c r="G217">
+        <v>1E-4</v>
+      </c>
+      <c r="H217">
+        <v>20</v>
+      </c>
+      <c r="I217">
+        <v>0</v>
+      </c>
+      <c r="J217">
+        <v>0</v>
+      </c>
+      <c r="K217">
+        <v>3.9676566067001442</v>
+      </c>
+      <c r="L217">
+        <v>9.79520592301024</v>
+      </c>
+      <c r="M217">
+        <v>123.9242907812329</v>
+      </c>
+      <c r="N217">
+        <v>0.31603329018816861</v>
+      </c>
+      <c r="O217">
+        <v>3.9676566067001429</v>
+      </c>
+      <c r="P217">
+        <v>11.666765339500641</v>
+      </c>
+      <c r="Q217">
+        <v>123.9242907812329</v>
+      </c>
+      <c r="R217">
+        <v>0.28928737983700792</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>234</v>
+      </c>
+      <c r="B218" t="b">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>52</v>
+      </c>
+      <c r="D218">
+        <v>12</v>
+      </c>
+      <c r="E218">
+        <v>32</v>
+      </c>
+      <c r="F218">
+        <v>8</v>
+      </c>
+      <c r="G218">
+        <v>1E-4</v>
+      </c>
+      <c r="H218">
+        <v>20</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+      <c r="J218">
+        <v>0</v>
+      </c>
+      <c r="K218">
+        <v>3.5888577541899669</v>
+      </c>
+      <c r="L218">
+        <v>8.8109845428619433</v>
+      </c>
+      <c r="M218">
+        <v>105.8969289471305</v>
+      </c>
+      <c r="N218">
+        <v>0.28332737169121341</v>
+      </c>
+      <c r="O218">
+        <v>3.588857754189966</v>
+      </c>
+      <c r="P218">
+        <v>10.441990155817059</v>
+      </c>
+      <c r="Q218">
+        <v>105.8969289471306</v>
+      </c>
+      <c r="R218">
+        <v>0.26505425586031528</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>235</v>
+      </c>
+      <c r="B219" t="b">
+        <v>1</v>
+      </c>
+      <c r="C219">
+        <v>52</v>
+      </c>
+      <c r="D219">
+        <v>3</v>
+      </c>
+      <c r="E219">
+        <v>64</v>
+      </c>
+      <c r="F219">
+        <v>8</v>
+      </c>
+      <c r="G219">
+        <v>1E-4</v>
+      </c>
+      <c r="H219">
+        <v>20</v>
+      </c>
+      <c r="I219">
+        <v>0</v>
+      </c>
+      <c r="J219">
+        <v>0</v>
+      </c>
+      <c r="K219">
+        <v>3.3363141583063101</v>
+      </c>
+      <c r="L219">
+        <v>8.3958930173489392</v>
+      </c>
+      <c r="M219">
+        <v>113.1349624678636</v>
+      </c>
+      <c r="N219">
+        <v>0.26917725094009348</v>
+      </c>
+      <c r="O219">
+        <v>3.3363141583063092</v>
+      </c>
+      <c r="P219">
+        <v>9.5718600181483726</v>
+      </c>
+      <c r="Q219">
+        <v>113.1349624678635</v>
+      </c>
+      <c r="R219">
+        <v>0.24059559392698701</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>236</v>
+      </c>
+      <c r="B220" t="b">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>52</v>
+      </c>
+      <c r="D220">
+        <v>6</v>
+      </c>
+      <c r="E220">
+        <v>64</v>
+      </c>
+      <c r="F220">
+        <v>8</v>
+      </c>
+      <c r="G220">
+        <v>1E-4</v>
+      </c>
+      <c r="H220">
+        <v>20</v>
+      </c>
+      <c r="I220">
+        <v>0</v>
+      </c>
+      <c r="J220">
+        <v>0</v>
+      </c>
+      <c r="K220">
+        <v>3.672164290961824</v>
+      </c>
+      <c r="L220">
+        <v>9.298060225256723</v>
+      </c>
+      <c r="M220">
+        <v>127.1135651296064</v>
+      </c>
+      <c r="N220">
+        <v>0.29313512813696813</v>
+      </c>
+      <c r="O220">
+        <v>3.6721642909618248</v>
+      </c>
+      <c r="P220">
+        <v>10.87118171975299</v>
+      </c>
+      <c r="Q220">
+        <v>127.1135651296065</v>
+      </c>
+      <c r="R220">
+        <v>0.26659295620944251</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>237</v>
+      </c>
+      <c r="B221" t="b">
+        <v>1</v>
+      </c>
+      <c r="C221">
+        <v>52</v>
+      </c>
+      <c r="D221">
+        <v>9</v>
+      </c>
+      <c r="E221">
+        <v>64</v>
+      </c>
+      <c r="F221">
+        <v>8</v>
+      </c>
+      <c r="G221">
+        <v>1E-4</v>
+      </c>
+      <c r="H221">
+        <v>20</v>
+      </c>
+      <c r="I221">
+        <v>0</v>
+      </c>
+      <c r="J221">
+        <v>0</v>
+      </c>
+      <c r="K221">
+        <v>3.6072189375270858</v>
+      </c>
+      <c r="L221">
+        <v>9.1073309746229167</v>
+      </c>
+      <c r="M221">
+        <v>119.0845696050164</v>
+      </c>
+      <c r="N221">
+        <v>0.29305400141488308</v>
+      </c>
+      <c r="O221">
+        <v>3.6072189375270871</v>
+      </c>
+      <c r="P221">
+        <v>10.664686063243339</v>
+      </c>
+      <c r="Q221">
+        <v>119.0845696050164</v>
+      </c>
+      <c r="R221">
+        <v>0.26274623755040039</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>238</v>
+      </c>
+      <c r="B222" t="b">
+        <v>1</v>
+      </c>
+      <c r="C222">
+        <v>52</v>
+      </c>
+      <c r="D222">
+        <v>12</v>
+      </c>
+      <c r="E222">
+        <v>64</v>
+      </c>
+      <c r="F222">
+        <v>8</v>
+      </c>
+      <c r="G222">
+        <v>1E-4</v>
+      </c>
+      <c r="H222">
+        <v>20</v>
+      </c>
+      <c r="I222">
+        <v>0</v>
+      </c>
+      <c r="J222">
+        <v>0</v>
+      </c>
+      <c r="K222">
+        <v>3.3733281627374518</v>
+      </c>
+      <c r="L222">
+        <v>8.6500534169852337</v>
+      </c>
+      <c r="M222">
+        <v>111.374864997751</v>
+      </c>
+      <c r="N222">
+        <v>0.27384538086046317</v>
+      </c>
+      <c r="O222">
+        <v>3.3733281627374518</v>
+      </c>
+      <c r="P222">
+        <v>10.197876164683461</v>
+      </c>
+      <c r="Q222">
+        <v>111.374864997751</v>
+      </c>
+      <c r="R222">
+        <v>0.24856499776772559</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>239</v>
+      </c>
+      <c r="B223" t="b">
+        <v>1</v>
+      </c>
+      <c r="C223">
+        <v>52</v>
+      </c>
+      <c r="D223">
+        <v>3</v>
+      </c>
+      <c r="E223">
+        <v>100</v>
+      </c>
+      <c r="F223">
+        <v>8</v>
+      </c>
+      <c r="G223">
+        <v>1E-4</v>
+      </c>
+      <c r="H223">
+        <v>20</v>
+      </c>
+      <c r="I223">
+        <v>0</v>
+      </c>
+      <c r="J223">
+        <v>0</v>
+      </c>
+      <c r="K223">
+        <v>3.3888008048403302</v>
+      </c>
+      <c r="L223">
+        <v>8.5585781382814652</v>
+      </c>
+      <c r="M223">
+        <v>115.84619178433699</v>
+      </c>
+      <c r="N223">
+        <v>0.27243014403774019</v>
+      </c>
+      <c r="O223">
+        <v>3.3888008048403289</v>
+      </c>
+      <c r="P223">
+        <v>9.7841079652038054</v>
+      </c>
+      <c r="Q223">
+        <v>115.84619178433709</v>
+      </c>
+      <c r="R223">
+        <v>0.24286129331350481</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>240</v>
+      </c>
+      <c r="B224" t="b">
+        <v>1</v>
+      </c>
+      <c r="C224">
+        <v>52</v>
+      </c>
+      <c r="D224">
+        <v>6</v>
+      </c>
+      <c r="E224">
+        <v>100</v>
+      </c>
+      <c r="F224">
+        <v>8</v>
+      </c>
+      <c r="G224">
+        <v>1E-4</v>
+      </c>
+      <c r="H224">
+        <v>20</v>
+      </c>
+      <c r="I224">
+        <v>0</v>
+      </c>
+      <c r="J224">
+        <v>0</v>
+      </c>
+      <c r="K224">
+        <v>3.693755935100012</v>
+      </c>
+      <c r="L224">
+        <v>9.614924457768252</v>
+      </c>
+      <c r="M224">
+        <v>139.8606775112768</v>
+      </c>
+      <c r="N224">
+        <v>0.29688283647827718</v>
+      </c>
+      <c r="O224">
+        <v>3.693755935100012</v>
+      </c>
+      <c r="P224">
+        <v>11.45045566989198</v>
+      </c>
+      <c r="Q224">
+        <v>139.8606775112768</v>
+      </c>
+      <c r="R224">
+        <v>0.26762081119302972</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>241</v>
+      </c>
+      <c r="B225" t="b">
+        <v>1</v>
+      </c>
+      <c r="C225">
+        <v>52</v>
+      </c>
+      <c r="D225">
+        <v>9</v>
+      </c>
+      <c r="E225">
+        <v>100</v>
+      </c>
+      <c r="F225">
+        <v>8</v>
+      </c>
+      <c r="G225">
+        <v>1E-4</v>
+      </c>
+      <c r="H225">
+        <v>20</v>
+      </c>
+      <c r="I225">
+        <v>0</v>
+      </c>
+      <c r="J225">
+        <v>0</v>
+      </c>
+      <c r="K225">
+        <v>3.5885669919220571</v>
+      </c>
+      <c r="L225">
+        <v>9.0035603077112132</v>
+      </c>
+      <c r="M225">
+        <v>121.0100210600356</v>
+      </c>
+      <c r="N225">
+        <v>0.28899942535295159</v>
+      </c>
+      <c r="O225">
+        <v>3.588566991922058</v>
+      </c>
+      <c r="P225">
+        <v>10.53616533110935</v>
+      </c>
+      <c r="Q225">
+        <v>121.0100210600356</v>
+      </c>
+      <c r="R225">
+        <v>0.2615265087929059</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>242</v>
+      </c>
+      <c r="B226" t="b">
+        <v>1</v>
+      </c>
+      <c r="C226">
+        <v>52</v>
+      </c>
+      <c r="D226">
+        <v>12</v>
+      </c>
+      <c r="E226">
+        <v>100</v>
+      </c>
+      <c r="F226">
+        <v>8</v>
+      </c>
+      <c r="G226">
+        <v>1E-4</v>
+      </c>
+      <c r="H226">
+        <v>20</v>
+      </c>
+      <c r="I226">
+        <v>0</v>
+      </c>
+      <c r="J226">
+        <v>0</v>
+      </c>
+      <c r="K226">
+        <v>3.7462692391262848</v>
+      </c>
+      <c r="L226">
+        <v>10.58850863891788</v>
+      </c>
+      <c r="M226">
+        <v>109.8086261727608</v>
+      </c>
+      <c r="N226">
+        <v>0.29794498858997559</v>
+      </c>
+      <c r="O226">
+        <v>3.7462692391262848</v>
+      </c>
+      <c r="P226">
+        <v>13.27609758880809</v>
+      </c>
+      <c r="Q226">
+        <v>109.8086261727609</v>
+      </c>
+      <c r="R226">
+        <v>0.27661026813659562</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>243</v>
+      </c>
+      <c r="B227" t="b">
+        <v>1</v>
+      </c>
+      <c r="C227">
+        <v>52</v>
+      </c>
+      <c r="D227">
+        <v>3</v>
+      </c>
+      <c r="E227">
+        <v>150</v>
+      </c>
+      <c r="F227">
+        <v>8</v>
+      </c>
+      <c r="G227">
+        <v>1E-4</v>
+      </c>
+      <c r="H227">
+        <v>20</v>
+      </c>
+      <c r="I227">
+        <v>0</v>
+      </c>
+      <c r="J227">
+        <v>0</v>
+      </c>
+      <c r="K227">
+        <v>3.3758274231670078</v>
+      </c>
+      <c r="L227">
+        <v>8.4665721156425935</v>
+      </c>
+      <c r="M227">
+        <v>112.3387699013944</v>
+      </c>
+      <c r="N227">
+        <v>0.26992950696408008</v>
+      </c>
+      <c r="O227">
+        <v>3.3758274231670078</v>
+      </c>
+      <c r="P227">
+        <v>9.6662224517178874</v>
+      </c>
+      <c r="Q227">
+        <v>112.3387699013944</v>
+      </c>
+      <c r="R227">
+        <v>0.24284836292416831</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>244</v>
+      </c>
+      <c r="B228" t="b">
+        <v>1</v>
+      </c>
+      <c r="C228">
+        <v>52</v>
+      </c>
+      <c r="D228">
+        <v>6</v>
+      </c>
+      <c r="E228">
+        <v>150</v>
+      </c>
+      <c r="F228">
+        <v>8</v>
+      </c>
+      <c r="G228">
+        <v>1E-4</v>
+      </c>
+      <c r="H228">
+        <v>20</v>
+      </c>
+      <c r="I228">
+        <v>0</v>
+      </c>
+      <c r="J228">
+        <v>0</v>
+      </c>
+      <c r="K228">
+        <v>3.596294730815234</v>
+      </c>
+      <c r="L228">
+        <v>9.0702406978359083</v>
+      </c>
+      <c r="M228">
+        <v>142.5138725587226</v>
+      </c>
+      <c r="N228">
+        <v>0.2910873421019301</v>
+      </c>
+      <c r="O228">
+        <v>3.596294730815234</v>
+      </c>
+      <c r="P228">
+        <v>10.565934038492991</v>
+      </c>
+      <c r="Q228">
+        <v>142.5138725587226</v>
+      </c>
+      <c r="R228">
+        <v>0.26093285758522361</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>245</v>
+      </c>
+      <c r="B229" t="b">
+        <v>1</v>
+      </c>
+      <c r="C229">
+        <v>52</v>
+      </c>
+      <c r="D229">
+        <v>9</v>
+      </c>
+      <c r="E229">
+        <v>150</v>
+      </c>
+      <c r="F229">
+        <v>8</v>
+      </c>
+      <c r="G229">
+        <v>1E-4</v>
+      </c>
+      <c r="H229">
+        <v>20</v>
+      </c>
+      <c r="I229">
+        <v>0</v>
+      </c>
+      <c r="J229">
+        <v>0</v>
+      </c>
+      <c r="K229">
+        <v>3.528394629604676</v>
+      </c>
+      <c r="L229">
+        <v>8.8128139482827699</v>
+      </c>
+      <c r="M229">
+        <v>115.4656780207262</v>
+      </c>
+      <c r="N229">
+        <v>0.28600463107691099</v>
+      </c>
+      <c r="O229">
+        <v>3.528394629604676</v>
+      </c>
+      <c r="P229">
+        <v>10.252308322931659</v>
+      </c>
+      <c r="Q229">
+        <v>115.4656780207262</v>
+      </c>
+      <c r="R229">
+        <v>0.25640025582875092</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>246</v>
+      </c>
+      <c r="B230" t="b">
+        <v>1</v>
+      </c>
+      <c r="C230">
+        <v>52</v>
+      </c>
+      <c r="D230">
+        <v>12</v>
+      </c>
+      <c r="E230">
+        <v>150</v>
+      </c>
+      <c r="F230">
+        <v>8</v>
+      </c>
+      <c r="G230">
+        <v>1E-4</v>
+      </c>
+      <c r="H230">
+        <v>20</v>
+      </c>
+      <c r="I230">
+        <v>0</v>
+      </c>
+      <c r="J230">
+        <v>0</v>
+      </c>
+      <c r="K230">
+        <v>3.5460209513395959</v>
+      </c>
+      <c r="L230">
+        <v>9.2518368114603593</v>
+      </c>
+      <c r="M230">
+        <v>107.4789689182701</v>
+      </c>
+      <c r="N230">
+        <v>0.28396497307009361</v>
+      </c>
+      <c r="O230">
+        <v>3.5460209513395959</v>
+      </c>
+      <c r="P230">
+        <v>11.11379612856617</v>
+      </c>
+      <c r="Q230">
+        <v>107.4789689182701</v>
+      </c>
+      <c r="R230">
+        <v>0.26109406788560002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>